<commit_message>
Data analysis for Biology completed
</commit_message>
<xml_diff>
--- a/Semester_3/Biology_Practicals/Observations/For_Oct1_2012_light.xlsx
+++ b/Semester_3/Biology_Practicals/Observations/For_Oct1_2012_light.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="6750"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="9675" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Vial2" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,11 @@
     <sheet name="Vial5" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="11">
   <si>
     <t>Vial 2 Light</t>
   </si>
@@ -53,6 +52,9 @@
   </si>
   <si>
     <t>&lt;&lt; One with food</t>
+  </si>
+  <si>
+    <t>G2</t>
   </si>
 </sst>
 </file>
@@ -394,28 +396,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -425,8 +436,19 @@
       <c r="C4">
         <v>52</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <f>SUM(B4,B8)</f>
+        <v>56</v>
+      </c>
+      <c r="H4">
+        <f>SUM(C4,C8)</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -436,8 +458,19 @@
       <c r="C5">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <f>SUM(B5,B9)</f>
+        <v>47</v>
+      </c>
+      <c r="H5">
+        <f>SUM(C5,C9)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>3</v>
       </c>
@@ -448,7 +481,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -459,7 +492,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -480,7 +513,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B3" sqref="B3:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,28 +560,34 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="H3" sqref="H3:I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -558,8 +597,19 @@
       <c r="C3">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <f>SUM(B3,B6)</f>
+        <v>15</v>
+      </c>
+      <c r="I3">
+        <f>SUM(C3,C6)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -569,8 +619,19 @@
       <c r="C4">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <f>SUM(B4,B7)</f>
+        <v>11</v>
+      </c>
+      <c r="I4">
+        <f>SUM(C4,C7)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -584,7 +645,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -604,8 +665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>